<commit_message>
add export and formate
</commit_message>
<xml_diff>
--- a/public/demo_files/Demo_FitnessDetails.xlsx
+++ b/public/demo_files/Demo_FitnessDetails.xlsx
@@ -4,7 +4,7 @@
   <fileVersion lastEdited="4" lowestEdited="4" rupBuild="3820"/>
   <workbookPr date1904="0"/>
   <bookViews>
-    <workbookView activeTab="0" windowWidth="10240" windowHeight="3450"/>
+    <workbookView activeTab="0" windowWidth="13660" windowHeight="5120"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -87,71 +87,130 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:S1"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0" tabSelected="1">
-      <selection activeCell="A2" sqref="A2:K2"/>
+    <sheetView workbookViewId="0" tabSelected="1">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" style="1" width="24.141406250000003" customWidth="1"/>
-    <col min="2" max="2" style="1" width="21.71298076923077" customWidth="1"/>
-    <col min="3" max="3" style="1" width="26.426983173076927" customWidth="1"/>
-    <col min="4" max="4" style="1" width="24.28425480769231" customWidth="1"/>
-    <col min="5" max="5" style="1" width="24.569951923076925" customWidth="1"/>
-    <col min="6" max="16384" style="1" width="9.142307692307693"/>
+    <col min="1" max="1" style="1" width="13.713461538461539" customWidth="1"/>
+    <col min="2" max="2" style="1" width="24.141406250000003" customWidth="1"/>
+    <col min="3" max="3" style="1" width="27.712620192307696" customWidth="1"/>
+    <col min="4" max="4" style="1" width="21.71298076923077" customWidth="1"/>
+    <col min="5" max="5" style="1" width="26.426983173076927" customWidth="1"/>
+    <col min="6" max="6" style="1" width="24.28425480769231" customWidth="1"/>
+    <col min="7" max="7" style="1" width="24.569951923076925" customWidth="1"/>
+    <col min="8" max="8" style="1" width="18.284615384615385" customWidth="1"/>
+    <col min="9" max="9" style="1" width="21.85582932692308" customWidth="1"/>
+    <col min="10" max="10" style="1" width="20.427343750000002" customWidth="1"/>
+    <col min="11" max="11" style="1" width="18.856009615384618" customWidth="1"/>
+    <col min="12" max="12" style="1" width="20.99873798076923" customWidth="1"/>
+    <col min="13" max="13" style="1" width="20.713040865384617" customWidth="1"/>
+    <col min="14" max="14" style="1" width="24.427103365384617" customWidth="1"/>
+    <col min="15" max="15" style="1" width="28.998257211538466" customWidth="1"/>
+    <col min="16" max="16" style="1" width="22.57007211538462" customWidth="1"/>
+    <col min="17" max="17" style="1" width="21.427283653846157" customWidth="1"/>
+    <col min="18" max="18" style="1" width="36.997776442307696" customWidth="1"/>
+    <col min="19" max="19" style="1" width="19.570252403846155" customWidth="1"/>
+    <col min="20" max="16384" style="1" width="9.142307692307693"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:19" ht="15">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Fleet Code</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>Vehicle Number</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Agent Name</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
         <is>
           <t>Fitness Number</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Fitness Amount </t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Payment Mode</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Pay Number</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Pay Date</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Pay Bank</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Pay Branch</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Valid From</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Valid Till</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Engine No.</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Chassis No</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>Manufacture Year</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Type Of Body</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>Type Of Fuel</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>Seating Capacity(including Driver)</t>
+        </is>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Cubic Capacity</t>
         </is>
       </c>
     </row>

</xml_diff>